<commit_message>
Remove the draft pdf extraction workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36061627-DB01-4569-98F1-97F63DEF4D6A}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADF68169-F52C-48EE-932B-B65502BFB4BB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1650,8 +1650,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Update contstants in config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADF68169-F52C-48EE-932B-B65502BFB4BB}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D87909CA-3D19-48C9-8B3B-04DE8B781481}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>01-1001-0000-91210-000-00000-00</t>
+  </si>
+  <si>
+    <t>NeedByDate</t>
+  </si>
+  <si>
+    <t>ProjectNo</t>
+  </si>
+  <si>
+    <t>FY24_0117_FTTB Rollout_01</t>
+  </si>
+  <si>
+    <t>Expenditure Date</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1666,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1867,9 +1879,24 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add to ToUpper and Trim in Short Partner Name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D87909CA-3D19-48C9-8B3B-04DE8B781481}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DB8121A-0CB5-4B27-BDCD-512982F29034}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
   </si>
   <si>
     <t>TaxClassificationCode</t>
@@ -580,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -630,9 +627,7 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1662,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1849,52 +1844,52 @@
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1"/>

</xml_diff>